<commit_message>
added the plan to the plan file
</commit_message>
<xml_diff>
--- a/tests/artifact/plan/GNUKhata-plan.xlsx
+++ b/tests/artifact/plan/GNUKhata-plan.xlsx
@@ -110,7 +110,7 @@
     <t>description of first plan step</t>
   </si>
   <si>
-    <t>UI-Settings</t>
+    <t>Mobile-Settings</t>
   </si>
   <si>
     <t>yes</t>
@@ -129,7 +129,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -202,13 +202,6 @@
       <color theme="7" tint="-0.499984740745262"/>
       <name val="Tahoma"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -787,146 +780,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1468,7 +1461,7 @@
   <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.5"/>

</xml_diff>